<commit_message>
Alpha 0.3.1 - Auto play on open, auto write on close
</commit_message>
<xml_diff>
--- a/Genre.xlsx
+++ b/Genre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Library_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F0FD4-3591-48E8-8358-85B7F2375169}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB8EB8-0D50-42BB-A92C-031A50D3C6ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E68DF470-1CD6-4F04-B000-D378EEF6E7F4}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>Drone</t>
   </si>
   <si>
-    <t>Funk</t>
-  </si>
-  <si>
     <t>UK</t>
   </si>
   <si>
@@ -165,13 +162,16 @@
     <t>Hardcore</t>
   </si>
   <si>
-    <t>Big-Beat</t>
-  </si>
-  <si>
     <t>Deep</t>
   </si>
   <si>
     <t>Hip-Hop</t>
+  </si>
+  <si>
+    <t>Big Beat</t>
+  </si>
+  <si>
+    <t>Funky</t>
   </si>
 </sst>
 </file>
@@ -530,7 +530,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -666,15 +666,15 @@
         <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -682,32 +682,32 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alpha 0.3.3 - Genre Update
</commit_message>
<xml_diff>
--- a/Genre.xlsx
+++ b/Genre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Library_Manager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\PycharmProjects\Library_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBB8EB8-0D50-42BB-A92C-031A50D3C6ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211B5D46-5C27-4382-B2CA-43B339B0BAA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E68DF470-1CD6-4F04-B000-D378EEF6E7F4}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{E68DF470-1CD6-4F04-B000-D378EEF6E7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Genre</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>Funky</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>Piano-house</t>
+  </si>
+  <si>
+    <t>Roller</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Jump-Up</t>
+  </si>
+  <si>
+    <t>Melodic</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Ambient</t>
   </si>
 </sst>
 </file>
@@ -207,12 +234,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB81966-232A-4466-BA73-40E43D7BC7D8}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +571,7 @@
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +584,11 @@
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -568,8 +601,11 @@
       <c r="D2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -583,7 +619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -597,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -611,7 +647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -625,7 +661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -635,8 +671,11 @@
       <c r="C7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -647,7 +686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -658,7 +697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -669,7 +708,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -680,7 +719,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -691,7 +730,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -702,12 +741,39 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>